<commit_message>
Put some fastq as example.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoiskroll/Dropbox/miseqUtils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F13609B-EDB4-5647-B85A-DE057F8BE593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7390AC4D-A60C-6B4C-80DB-F4C4F197B405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2820" windowWidth="27240" windowHeight="16120" xr2:uid="{0A4B0C7D-21C4-F44C-B1D6-C1767AAEA4B0}"/>
   </bookViews>
@@ -46,10 +46,10 @@
     <t>exampleRef.fa</t>
   </si>
   <si>
-    <t>A01</t>
+    <t>D01</t>
   </si>
   <si>
-    <t>A11</t>
+    <t>D11</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>